<commit_message>
testing new data set
</commit_message>
<xml_diff>
--- a/Creatures.xlsx
+++ b/Creatures.xlsx
@@ -5,16 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tay042919\ML_Playground\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ML_Playground_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CC1DD5FA-A218-4041-96E9-7CC40E1548F4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98F222A1-86F2-487F-AF79-822A899A3A39}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-2370" windowWidth="29040" windowHeight="15840" xr2:uid="{4A1C3A05-E704-44DB-95C2-CD911D50CE24}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$F$1:$F$251</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="10">
   <si>
     <t>Type</t>
   </si>
@@ -413,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DB04430-3042-43D2-B6BA-A1963861CABC}">
-  <dimension ref="A1:L126"/>
+  <dimension ref="A1:L251"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H106" sqref="H106:I108"/>
+    <sheetView tabSelected="1" topLeftCell="A211" workbookViewId="0">
+      <selection activeCell="I232" sqref="I232:K235"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -750,7 +753,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -769,8 +772,9 @@
       <c r="F17" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -790,7 +794,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -810,7 +814,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -830,7 +834,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -850,7 +854,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -870,7 +874,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -890,7 +894,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -910,7 +914,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -930,7 +934,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -950,7 +954,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -970,7 +974,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -990,7 +994,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1010,7 +1014,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1030,7 +1034,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1050,7 +1054,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2957,7 +2961,2511 @@
         <v>9</v>
       </c>
     </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A127">
+        <v>126</v>
+      </c>
+      <c r="B127">
+        <v>0</v>
+      </c>
+      <c r="C127">
+        <v>0</v>
+      </c>
+      <c r="D127">
+        <v>118</v>
+      </c>
+      <c r="E127">
+        <v>14</v>
+      </c>
+      <c r="F127" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A128">
+        <v>127</v>
+      </c>
+      <c r="B128">
+        <v>0</v>
+      </c>
+      <c r="C128">
+        <v>0</v>
+      </c>
+      <c r="D128">
+        <v>113</v>
+      </c>
+      <c r="E128">
+        <v>22</v>
+      </c>
+      <c r="F128" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A129">
+        <v>128</v>
+      </c>
+      <c r="B129">
+        <v>0</v>
+      </c>
+      <c r="C129">
+        <v>2</v>
+      </c>
+      <c r="D129">
+        <v>176</v>
+      </c>
+      <c r="E129">
+        <v>15</v>
+      </c>
+      <c r="F129" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A130">
+        <v>129</v>
+      </c>
+      <c r="B130">
+        <v>4</v>
+      </c>
+      <c r="C130">
+        <v>4</v>
+      </c>
+      <c r="D130">
+        <v>74</v>
+      </c>
+      <c r="E130">
+        <v>49</v>
+      </c>
+      <c r="F130" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A131">
+        <v>130</v>
+      </c>
+      <c r="B131">
+        <v>4</v>
+      </c>
+      <c r="C131">
+        <v>2</v>
+      </c>
+      <c r="D131">
+        <v>72</v>
+      </c>
+      <c r="E131">
+        <v>45</v>
+      </c>
+      <c r="F131" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A132">
+        <v>131</v>
+      </c>
+      <c r="B132">
+        <v>4</v>
+      </c>
+      <c r="C132">
+        <v>6</v>
+      </c>
+      <c r="D132">
+        <v>65</v>
+      </c>
+      <c r="E132">
+        <v>42</v>
+      </c>
+      <c r="F132" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A133">
+        <v>132</v>
+      </c>
+      <c r="B133">
+        <v>2</v>
+      </c>
+      <c r="C133">
+        <v>2</v>
+      </c>
+      <c r="D133">
+        <v>25</v>
+      </c>
+      <c r="E133">
+        <v>68</v>
+      </c>
+      <c r="F133" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A134">
+        <v>133</v>
+      </c>
+      <c r="B134">
+        <v>4</v>
+      </c>
+      <c r="C134">
+        <v>0</v>
+      </c>
+      <c r="D134">
+        <v>101</v>
+      </c>
+      <c r="E134">
+        <v>18</v>
+      </c>
+      <c r="F134" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A135">
+        <v>134</v>
+      </c>
+      <c r="B135">
+        <v>2</v>
+      </c>
+      <c r="C135">
+        <v>2</v>
+      </c>
+      <c r="D135">
+        <v>21</v>
+      </c>
+      <c r="E135">
+        <v>88</v>
+      </c>
+      <c r="F135" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A136">
+        <v>135</v>
+      </c>
+      <c r="B136">
+        <v>4</v>
+      </c>
+      <c r="C136">
+        <v>6</v>
+      </c>
+      <c r="D136">
+        <v>72</v>
+      </c>
+      <c r="E136">
+        <v>48</v>
+      </c>
+      <c r="F136" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A137">
+        <v>136</v>
+      </c>
+      <c r="B137">
+        <v>0</v>
+      </c>
+      <c r="C137">
+        <v>0</v>
+      </c>
+      <c r="D137">
+        <v>119</v>
+      </c>
+      <c r="E137">
+        <v>15</v>
+      </c>
+      <c r="F137" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A138">
+        <v>137</v>
+      </c>
+      <c r="B138">
+        <v>0</v>
+      </c>
+      <c r="C138">
+        <v>0</v>
+      </c>
+      <c r="D138">
+        <v>112</v>
+      </c>
+      <c r="E138">
+        <v>13</v>
+      </c>
+      <c r="F138" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A139">
+        <v>138</v>
+      </c>
+      <c r="B139">
+        <v>0</v>
+      </c>
+      <c r="C139">
+        <v>2</v>
+      </c>
+      <c r="D139">
+        <v>156</v>
+      </c>
+      <c r="E139">
+        <v>8</v>
+      </c>
+      <c r="F139" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A140">
+        <v>139</v>
+      </c>
+      <c r="B140">
+        <v>4</v>
+      </c>
+      <c r="C140">
+        <v>4</v>
+      </c>
+      <c r="D140">
+        <v>66</v>
+      </c>
+      <c r="E140">
+        <v>42</v>
+      </c>
+      <c r="F140" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A141">
+        <v>140</v>
+      </c>
+      <c r="B141">
+        <v>2</v>
+      </c>
+      <c r="C141">
+        <v>2</v>
+      </c>
+      <c r="D141">
+        <v>18</v>
+      </c>
+      <c r="E141">
+        <v>80</v>
+      </c>
+      <c r="F141" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A142">
+        <v>141</v>
+      </c>
+      <c r="B142">
+        <v>0</v>
+      </c>
+      <c r="C142">
+        <v>0</v>
+      </c>
+      <c r="D142">
+        <v>98</v>
+      </c>
+      <c r="E142">
+        <v>18</v>
+      </c>
+      <c r="F142" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A143">
+        <v>142</v>
+      </c>
+      <c r="B143">
+        <v>4</v>
+      </c>
+      <c r="C143">
+        <v>6</v>
+      </c>
+      <c r="D143">
+        <v>79</v>
+      </c>
+      <c r="E143">
+        <v>50</v>
+      </c>
+      <c r="F143" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A144">
+        <v>143</v>
+      </c>
+      <c r="B144">
+        <v>0</v>
+      </c>
+      <c r="C144">
+        <v>0</v>
+      </c>
+      <c r="D144">
+        <v>121</v>
+      </c>
+      <c r="E144">
+        <v>15</v>
+      </c>
+      <c r="F144" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A145">
+        <v>144</v>
+      </c>
+      <c r="B145">
+        <v>0</v>
+      </c>
+      <c r="C145">
+        <v>2</v>
+      </c>
+      <c r="D145">
+        <v>188</v>
+      </c>
+      <c r="E145">
+        <v>8</v>
+      </c>
+      <c r="F145" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A146">
+        <v>145</v>
+      </c>
+      <c r="B146">
+        <v>0</v>
+      </c>
+      <c r="C146">
+        <v>2</v>
+      </c>
+      <c r="D146">
+        <v>154</v>
+      </c>
+      <c r="E146">
+        <v>5</v>
+      </c>
+      <c r="F146" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A147">
+        <v>146</v>
+      </c>
+      <c r="B147">
+        <v>4</v>
+      </c>
+      <c r="C147">
+        <v>4</v>
+      </c>
+      <c r="D147">
+        <v>82</v>
+      </c>
+      <c r="E147">
+        <v>45</v>
+      </c>
+      <c r="F147" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A148">
+        <v>147</v>
+      </c>
+      <c r="B148">
+        <v>0</v>
+      </c>
+      <c r="C148">
+        <v>0</v>
+      </c>
+      <c r="D148">
+        <v>130</v>
+      </c>
+      <c r="E148">
+        <v>19</v>
+      </c>
+      <c r="F148" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A149">
+        <v>148</v>
+      </c>
+      <c r="B149">
+        <v>2</v>
+      </c>
+      <c r="C149">
+        <v>2</v>
+      </c>
+      <c r="D149">
+        <v>18</v>
+      </c>
+      <c r="E149">
+        <v>80</v>
+      </c>
+      <c r="F149" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A150">
+        <v>149</v>
+      </c>
+      <c r="B150">
+        <v>2</v>
+      </c>
+      <c r="C150">
+        <v>2</v>
+      </c>
+      <c r="D150">
+        <v>25</v>
+      </c>
+      <c r="E150">
+        <v>95</v>
+      </c>
+      <c r="F150" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A151">
+        <v>150</v>
+      </c>
+      <c r="B151">
+        <v>2</v>
+      </c>
+      <c r="C151">
+        <v>2</v>
+      </c>
+      <c r="D151">
+        <v>32</v>
+      </c>
+      <c r="E151">
+        <v>88</v>
+      </c>
+      <c r="F151" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A152">
+        <v>151</v>
+      </c>
+      <c r="B152">
+        <v>0</v>
+      </c>
+      <c r="C152">
+        <v>0</v>
+      </c>
+      <c r="D152">
+        <v>127</v>
+      </c>
+      <c r="E152">
+        <v>19</v>
+      </c>
+      <c r="F152" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A153">
+        <v>152</v>
+      </c>
+      <c r="B153">
+        <v>0</v>
+      </c>
+      <c r="C153">
+        <v>2</v>
+      </c>
+      <c r="D153">
+        <v>165</v>
+      </c>
+      <c r="E153">
+        <v>5</v>
+      </c>
+      <c r="F153" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A154">
+        <v>153</v>
+      </c>
+      <c r="B154">
+        <v>4</v>
+      </c>
+      <c r="C154">
+        <v>4</v>
+      </c>
+      <c r="D154">
+        <v>72</v>
+      </c>
+      <c r="E154">
+        <v>60</v>
+      </c>
+      <c r="F154" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A155">
+        <v>154</v>
+      </c>
+      <c r="B155">
+        <v>2</v>
+      </c>
+      <c r="C155">
+        <v>2</v>
+      </c>
+      <c r="D155">
+        <v>25</v>
+      </c>
+      <c r="E155">
+        <v>80</v>
+      </c>
+      <c r="F155" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A156">
+        <v>155</v>
+      </c>
+      <c r="B156">
+        <v>2</v>
+      </c>
+      <c r="C156">
+        <v>2</v>
+      </c>
+      <c r="D156">
+        <v>28</v>
+      </c>
+      <c r="E156">
+        <v>100</v>
+      </c>
+      <c r="F156" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A157">
+        <v>156</v>
+      </c>
+      <c r="B157">
+        <v>4</v>
+      </c>
+      <c r="C157">
+        <v>4</v>
+      </c>
+      <c r="D157">
+        <v>42</v>
+      </c>
+      <c r="E157">
+        <v>30</v>
+      </c>
+      <c r="F157" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A158">
+        <v>157</v>
+      </c>
+      <c r="B158">
+        <v>0</v>
+      </c>
+      <c r="C158">
+        <v>2</v>
+      </c>
+      <c r="D158">
+        <v>196</v>
+      </c>
+      <c r="E158">
+        <v>9</v>
+      </c>
+      <c r="F158" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A159">
+        <v>158</v>
+      </c>
+      <c r="B159">
+        <v>4</v>
+      </c>
+      <c r="C159">
+        <v>6</v>
+      </c>
+      <c r="D159">
+        <v>88</v>
+      </c>
+      <c r="E159">
+        <v>45</v>
+      </c>
+      <c r="F159" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A160">
+        <v>159</v>
+      </c>
+      <c r="B160">
+        <v>2</v>
+      </c>
+      <c r="C160">
+        <v>2</v>
+      </c>
+      <c r="D160">
+        <v>25</v>
+      </c>
+      <c r="E160">
+        <v>140</v>
+      </c>
+      <c r="F160" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="161" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A161">
+        <v>160</v>
+      </c>
+      <c r="B161">
+        <v>0</v>
+      </c>
+      <c r="C161">
+        <v>0</v>
+      </c>
+      <c r="D161">
+        <v>112</v>
+      </c>
+      <c r="E161">
+        <v>18</v>
+      </c>
+      <c r="F161" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="162" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A162">
+        <v>161</v>
+      </c>
+      <c r="B162">
+        <v>0</v>
+      </c>
+      <c r="C162">
+        <v>0</v>
+      </c>
+      <c r="D162">
+        <v>89</v>
+      </c>
+      <c r="E162">
+        <v>12</v>
+      </c>
+      <c r="F162" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="163" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A163">
+        <v>162</v>
+      </c>
+      <c r="B163">
+        <v>0</v>
+      </c>
+      <c r="C163">
+        <v>2</v>
+      </c>
+      <c r="D163">
+        <v>158</v>
+      </c>
+      <c r="E163">
+        <v>6</v>
+      </c>
+      <c r="F163" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="164" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A164">
+        <v>163</v>
+      </c>
+      <c r="B164">
+        <v>0</v>
+      </c>
+      <c r="C164">
+        <v>0</v>
+      </c>
+      <c r="D164">
+        <v>140</v>
+      </c>
+      <c r="E164">
+        <v>18</v>
+      </c>
+      <c r="F164" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="165" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A165">
+        <v>164</v>
+      </c>
+      <c r="B165">
+        <v>2</v>
+      </c>
+      <c r="C165">
+        <v>2</v>
+      </c>
+      <c r="D165">
+        <v>25</v>
+      </c>
+      <c r="E165">
+        <v>105</v>
+      </c>
+      <c r="F165" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="166" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A166">
+        <v>165</v>
+      </c>
+      <c r="B166">
+        <v>4</v>
+      </c>
+      <c r="C166">
+        <v>6</v>
+      </c>
+      <c r="D166">
+        <v>79</v>
+      </c>
+      <c r="E166">
+        <v>45</v>
+      </c>
+      <c r="F166" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="167" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A167">
+        <v>166</v>
+      </c>
+      <c r="B167">
+        <v>4</v>
+      </c>
+      <c r="C167">
+        <v>4</v>
+      </c>
+      <c r="D167">
+        <v>80</v>
+      </c>
+      <c r="E167">
+        <v>42</v>
+      </c>
+      <c r="F167" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="168" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A168">
+        <v>167</v>
+      </c>
+      <c r="B168">
+        <v>4</v>
+      </c>
+      <c r="C168">
+        <v>0</v>
+      </c>
+      <c r="D168">
+        <v>131</v>
+      </c>
+      <c r="E168">
+        <v>18</v>
+      </c>
+      <c r="F168" t="s">
+        <v>8</v>
+      </c>
+      <c r="J168" s="1"/>
+    </row>
+    <row r="169" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A169">
+        <v>168</v>
+      </c>
+      <c r="B169">
+        <v>4</v>
+      </c>
+      <c r="C169">
+        <v>2</v>
+      </c>
+      <c r="D169">
+        <v>45</v>
+      </c>
+      <c r="E169">
+        <v>30</v>
+      </c>
+      <c r="F169" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="170" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A170">
+        <v>169</v>
+      </c>
+      <c r="B170">
+        <v>0</v>
+      </c>
+      <c r="C170">
+        <v>2</v>
+      </c>
+      <c r="D170">
+        <v>192</v>
+      </c>
+      <c r="E170">
+        <v>8</v>
+      </c>
+      <c r="F170" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="171" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A171">
+        <v>170</v>
+      </c>
+      <c r="B171">
+        <v>2</v>
+      </c>
+      <c r="C171">
+        <v>2</v>
+      </c>
+      <c r="D171">
+        <v>24</v>
+      </c>
+      <c r="E171">
+        <v>88</v>
+      </c>
+      <c r="F171" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="172" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A172">
+        <v>171</v>
+      </c>
+      <c r="B172">
+        <v>4</v>
+      </c>
+      <c r="C172">
+        <v>4</v>
+      </c>
+      <c r="D172">
+        <v>62</v>
+      </c>
+      <c r="E172">
+        <v>40</v>
+      </c>
+      <c r="F172" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="173" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A173">
+        <v>172</v>
+      </c>
+      <c r="B173">
+        <v>0</v>
+      </c>
+      <c r="C173">
+        <v>0</v>
+      </c>
+      <c r="D173">
+        <v>139</v>
+      </c>
+      <c r="E173">
+        <v>20</v>
+      </c>
+      <c r="F173" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="174" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A174">
+        <v>173</v>
+      </c>
+      <c r="B174">
+        <v>2</v>
+      </c>
+      <c r="C174">
+        <v>2</v>
+      </c>
+      <c r="D174">
+        <v>22</v>
+      </c>
+      <c r="E174">
+        <v>92</v>
+      </c>
+      <c r="F174" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="175" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A175">
+        <v>174</v>
+      </c>
+      <c r="B175">
+        <v>2</v>
+      </c>
+      <c r="C175">
+        <v>2</v>
+      </c>
+      <c r="D175">
+        <v>24</v>
+      </c>
+      <c r="E175">
+        <v>106</v>
+      </c>
+      <c r="F175" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="176" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A176">
+        <v>175</v>
+      </c>
+      <c r="B176">
+        <v>0</v>
+      </c>
+      <c r="C176">
+        <v>0</v>
+      </c>
+      <c r="D176">
+        <v>118</v>
+      </c>
+      <c r="E176">
+        <v>18</v>
+      </c>
+      <c r="F176" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="177" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A177">
+        <v>176</v>
+      </c>
+      <c r="B177">
+        <v>0</v>
+      </c>
+      <c r="C177">
+        <v>2</v>
+      </c>
+      <c r="D177">
+        <v>122</v>
+      </c>
+      <c r="E177">
+        <v>6</v>
+      </c>
+      <c r="F177" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="178" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A178">
+        <v>177</v>
+      </c>
+      <c r="B178">
+        <v>0</v>
+      </c>
+      <c r="C178">
+        <v>4</v>
+      </c>
+      <c r="D178">
+        <v>176</v>
+      </c>
+      <c r="E178">
+        <v>6</v>
+      </c>
+      <c r="F178" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="179" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A179">
+        <v>178</v>
+      </c>
+      <c r="B179">
+        <v>0</v>
+      </c>
+      <c r="C179">
+        <v>0</v>
+      </c>
+      <c r="D179">
+        <v>120</v>
+      </c>
+      <c r="E179">
+        <v>12</v>
+      </c>
+      <c r="F179" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="180" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A180">
+        <v>179</v>
+      </c>
+      <c r="B180">
+        <v>4</v>
+      </c>
+      <c r="C180">
+        <v>4</v>
+      </c>
+      <c r="D180">
+        <v>42</v>
+      </c>
+      <c r="E180">
+        <v>30</v>
+      </c>
+      <c r="F180" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="181" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A181">
+        <v>180</v>
+      </c>
+      <c r="B181">
+        <v>0</v>
+      </c>
+      <c r="C181">
+        <v>2</v>
+      </c>
+      <c r="D181">
+        <v>182</v>
+      </c>
+      <c r="E181">
+        <v>8</v>
+      </c>
+      <c r="F181" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="182" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A182">
+        <v>181</v>
+      </c>
+      <c r="B182">
+        <v>2</v>
+      </c>
+      <c r="C182">
+        <v>2</v>
+      </c>
+      <c r="D182">
+        <v>18</v>
+      </c>
+      <c r="E182">
+        <v>60</v>
+      </c>
+      <c r="F182" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="183" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A183">
+        <v>182</v>
+      </c>
+      <c r="B183">
+        <v>4</v>
+      </c>
+      <c r="C183">
+        <v>4</v>
+      </c>
+      <c r="D183">
+        <v>45</v>
+      </c>
+      <c r="E183">
+        <v>45</v>
+      </c>
+      <c r="F183" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="184" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A184">
+        <v>183</v>
+      </c>
+      <c r="B184">
+        <v>2</v>
+      </c>
+      <c r="C184">
+        <v>2</v>
+      </c>
+      <c r="D184">
+        <v>18</v>
+      </c>
+      <c r="E184">
+        <v>60</v>
+      </c>
+      <c r="F184" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="185" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A185">
+        <v>184</v>
+      </c>
+      <c r="B185">
+        <v>4</v>
+      </c>
+      <c r="C185">
+        <v>0</v>
+      </c>
+      <c r="D185">
+        <v>99</v>
+      </c>
+      <c r="E185">
+        <v>15</v>
+      </c>
+      <c r="F185" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="186" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A186">
+        <v>185</v>
+      </c>
+      <c r="B186">
+        <v>2</v>
+      </c>
+      <c r="C186">
+        <v>2</v>
+      </c>
+      <c r="D186">
+        <v>20</v>
+      </c>
+      <c r="E186">
+        <v>80</v>
+      </c>
+      <c r="F186" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="187" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A187">
+        <v>186</v>
+      </c>
+      <c r="B187">
+        <v>0</v>
+      </c>
+      <c r="C187">
+        <v>0</v>
+      </c>
+      <c r="D187">
+        <v>118</v>
+      </c>
+      <c r="E187">
+        <v>18</v>
+      </c>
+      <c r="F187" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="188" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A188">
+        <v>187</v>
+      </c>
+      <c r="B188">
+        <v>0</v>
+      </c>
+      <c r="C188">
+        <v>4</v>
+      </c>
+      <c r="D188">
+        <v>192</v>
+      </c>
+      <c r="E188">
+        <v>6</v>
+      </c>
+      <c r="F188" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="189" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A189">
+        <v>188</v>
+      </c>
+      <c r="B189">
+        <v>0</v>
+      </c>
+      <c r="C189">
+        <v>0</v>
+      </c>
+      <c r="D189">
+        <v>127</v>
+      </c>
+      <c r="E189">
+        <v>17</v>
+      </c>
+      <c r="F189" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="190" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A190">
+        <v>189</v>
+      </c>
+      <c r="B190">
+        <v>2</v>
+      </c>
+      <c r="C190">
+        <v>2</v>
+      </c>
+      <c r="D190">
+        <v>25</v>
+      </c>
+      <c r="E190">
+        <v>80</v>
+      </c>
+      <c r="F190" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="191" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A191">
+        <v>190</v>
+      </c>
+      <c r="B191">
+        <v>0</v>
+      </c>
+      <c r="C191">
+        <v>2</v>
+      </c>
+      <c r="D191">
+        <v>188</v>
+      </c>
+      <c r="E191">
+        <v>8</v>
+      </c>
+      <c r="F191" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="192" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A192">
+        <v>191</v>
+      </c>
+      <c r="B192">
+        <v>0</v>
+      </c>
+      <c r="C192">
+        <v>2</v>
+      </c>
+      <c r="D192">
+        <v>192</v>
+      </c>
+      <c r="E192">
+        <v>8</v>
+      </c>
+      <c r="F192" t="s">
+        <v>9</v>
+      </c>
+      <c r="J192" s="1"/>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A193">
+        <v>192</v>
+      </c>
+      <c r="B193">
+        <v>0</v>
+      </c>
+      <c r="C193">
+        <v>0</v>
+      </c>
+      <c r="D193">
+        <v>120</v>
+      </c>
+      <c r="E193">
+        <v>16</v>
+      </c>
+      <c r="F193" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A194">
+        <v>193</v>
+      </c>
+      <c r="B194">
+        <v>4</v>
+      </c>
+      <c r="C194">
+        <v>2</v>
+      </c>
+      <c r="D194">
+        <v>42</v>
+      </c>
+      <c r="E194">
+        <v>32</v>
+      </c>
+      <c r="F194" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A195">
+        <v>194</v>
+      </c>
+      <c r="B195">
+        <v>4</v>
+      </c>
+      <c r="C195">
+        <v>2</v>
+      </c>
+      <c r="D195">
+        <v>55</v>
+      </c>
+      <c r="E195">
+        <v>35</v>
+      </c>
+      <c r="F195" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A196">
+        <v>195</v>
+      </c>
+      <c r="B196">
+        <v>4</v>
+      </c>
+      <c r="C196">
+        <v>4</v>
+      </c>
+      <c r="D196">
+        <v>74</v>
+      </c>
+      <c r="E196">
+        <v>40</v>
+      </c>
+      <c r="F196" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A197">
+        <v>196</v>
+      </c>
+      <c r="B197">
+        <v>0</v>
+      </c>
+      <c r="C197">
+        <v>0</v>
+      </c>
+      <c r="D197">
+        <v>115</v>
+      </c>
+      <c r="E197">
+        <v>11</v>
+      </c>
+      <c r="F197" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A198">
+        <v>197</v>
+      </c>
+      <c r="B198">
+        <v>4</v>
+      </c>
+      <c r="C198">
+        <v>2</v>
+      </c>
+      <c r="D198">
+        <v>72</v>
+      </c>
+      <c r="E198">
+        <v>41</v>
+      </c>
+      <c r="F198" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A199">
+        <v>198</v>
+      </c>
+      <c r="B199">
+        <v>4</v>
+      </c>
+      <c r="C199">
+        <v>2</v>
+      </c>
+      <c r="D199">
+        <v>69</v>
+      </c>
+      <c r="E199">
+        <v>40</v>
+      </c>
+      <c r="F199" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A200">
+        <v>199</v>
+      </c>
+      <c r="B200">
+        <v>0</v>
+      </c>
+      <c r="C200">
+        <v>0</v>
+      </c>
+      <c r="D200">
+        <v>121</v>
+      </c>
+      <c r="E200">
+        <v>20</v>
+      </c>
+      <c r="F200" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A201">
+        <v>200</v>
+      </c>
+      <c r="B201">
+        <v>2</v>
+      </c>
+      <c r="C201">
+        <v>2</v>
+      </c>
+      <c r="D201">
+        <v>25</v>
+      </c>
+      <c r="E201">
+        <v>62</v>
+      </c>
+      <c r="F201" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A202">
+        <v>201</v>
+      </c>
+      <c r="B202">
+        <v>4</v>
+      </c>
+      <c r="C202">
+        <v>4</v>
+      </c>
+      <c r="D202">
+        <v>80</v>
+      </c>
+      <c r="E202">
+        <v>42</v>
+      </c>
+      <c r="F202" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A203">
+        <v>202</v>
+      </c>
+      <c r="B203">
+        <v>0</v>
+      </c>
+      <c r="C203">
+        <v>0</v>
+      </c>
+      <c r="D203">
+        <v>109</v>
+      </c>
+      <c r="E203">
+        <v>18</v>
+      </c>
+      <c r="F203" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A204">
+        <v>203</v>
+      </c>
+      <c r="B204">
+        <v>0</v>
+      </c>
+      <c r="C204">
+        <v>4</v>
+      </c>
+      <c r="D204">
+        <v>152</v>
+      </c>
+      <c r="E204">
+        <v>5</v>
+      </c>
+      <c r="F204" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A205">
+        <v>204</v>
+      </c>
+      <c r="B205">
+        <v>2</v>
+      </c>
+      <c r="C205">
+        <v>2</v>
+      </c>
+      <c r="D205">
+        <v>50</v>
+      </c>
+      <c r="E205">
+        <v>150</v>
+      </c>
+      <c r="F205" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A206">
+        <v>205</v>
+      </c>
+      <c r="B206">
+        <v>4</v>
+      </c>
+      <c r="C206">
+        <v>2</v>
+      </c>
+      <c r="D206">
+        <v>75</v>
+      </c>
+      <c r="E206">
+        <v>45</v>
+      </c>
+      <c r="F206" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A207">
+        <v>206</v>
+      </c>
+      <c r="B207">
+        <v>0</v>
+      </c>
+      <c r="C207">
+        <v>2</v>
+      </c>
+      <c r="D207">
+        <v>145</v>
+      </c>
+      <c r="E207">
+        <v>10</v>
+      </c>
+      <c r="F207" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A208">
+        <v>207</v>
+      </c>
+      <c r="B208">
+        <v>2</v>
+      </c>
+      <c r="C208">
+        <v>2</v>
+      </c>
+      <c r="D208">
+        <v>22</v>
+      </c>
+      <c r="E208">
+        <v>80</v>
+      </c>
+      <c r="F208" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A209">
+        <v>208</v>
+      </c>
+      <c r="B209">
+        <v>2</v>
+      </c>
+      <c r="C209">
+        <v>2</v>
+      </c>
+      <c r="D209">
+        <v>32</v>
+      </c>
+      <c r="E209">
+        <v>96</v>
+      </c>
+      <c r="F209" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A210">
+        <v>209</v>
+      </c>
+      <c r="B210">
+        <v>0</v>
+      </c>
+      <c r="C210">
+        <v>2</v>
+      </c>
+      <c r="D210">
+        <v>188</v>
+      </c>
+      <c r="E210">
+        <v>18</v>
+      </c>
+      <c r="F210" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A211">
+        <v>210</v>
+      </c>
+      <c r="B211">
+        <v>4</v>
+      </c>
+      <c r="C211">
+        <v>6</v>
+      </c>
+      <c r="D211">
+        <v>78</v>
+      </c>
+      <c r="E211">
+        <v>48</v>
+      </c>
+      <c r="F211" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A212">
+        <v>211</v>
+      </c>
+      <c r="B212">
+        <v>4</v>
+      </c>
+      <c r="C212">
+        <v>4</v>
+      </c>
+      <c r="D212">
+        <v>82</v>
+      </c>
+      <c r="E212">
+        <v>48</v>
+      </c>
+      <c r="F212" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A213">
+        <v>212</v>
+      </c>
+      <c r="B213">
+        <v>4</v>
+      </c>
+      <c r="C213">
+        <v>2</v>
+      </c>
+      <c r="D213">
+        <v>66</v>
+      </c>
+      <c r="E213">
+        <v>36</v>
+      </c>
+      <c r="F213" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A214">
+        <v>213</v>
+      </c>
+      <c r="B214">
+        <v>4</v>
+      </c>
+      <c r="C214">
+        <v>6</v>
+      </c>
+      <c r="D214">
+        <v>80</v>
+      </c>
+      <c r="E214">
+        <v>40</v>
+      </c>
+      <c r="F214" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A215">
+        <v>214</v>
+      </c>
+      <c r="B215">
+        <v>2</v>
+      </c>
+      <c r="C215">
+        <v>2</v>
+      </c>
+      <c r="D215">
+        <v>42</v>
+      </c>
+      <c r="E215">
+        <v>109</v>
+      </c>
+      <c r="F215" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A216">
+        <v>215</v>
+      </c>
+      <c r="B216">
+        <v>4</v>
+      </c>
+      <c r="C216">
+        <v>6</v>
+      </c>
+      <c r="D216">
+        <v>85</v>
+      </c>
+      <c r="E216">
+        <v>50</v>
+      </c>
+      <c r="F216" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A217">
+        <v>216</v>
+      </c>
+      <c r="B217">
+        <v>0</v>
+      </c>
+      <c r="C217">
+        <v>0</v>
+      </c>
+      <c r="D217">
+        <v>139</v>
+      </c>
+      <c r="E217">
+        <v>20</v>
+      </c>
+      <c r="F217" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A218">
+        <v>217</v>
+      </c>
+      <c r="B218">
+        <v>0</v>
+      </c>
+      <c r="C218">
+        <v>2</v>
+      </c>
+      <c r="D218">
+        <v>198</v>
+      </c>
+      <c r="E218">
+        <v>18</v>
+      </c>
+      <c r="F218" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A219">
+        <v>218</v>
+      </c>
+      <c r="B219">
+        <v>4</v>
+      </c>
+      <c r="C219">
+        <v>4</v>
+      </c>
+      <c r="D219">
+        <v>42</v>
+      </c>
+      <c r="E219">
+        <v>39</v>
+      </c>
+      <c r="F219" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A220">
+        <v>219</v>
+      </c>
+      <c r="B220">
+        <v>0</v>
+      </c>
+      <c r="C220">
+        <v>2</v>
+      </c>
+      <c r="D220">
+        <v>139</v>
+      </c>
+      <c r="E220">
+        <v>18</v>
+      </c>
+      <c r="F220" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A221">
+        <v>220</v>
+      </c>
+      <c r="B221">
+        <v>0</v>
+      </c>
+      <c r="C221">
+        <v>0</v>
+      </c>
+      <c r="D221">
+        <v>118</v>
+      </c>
+      <c r="E221">
+        <v>22</v>
+      </c>
+      <c r="F221" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A222">
+        <v>221</v>
+      </c>
+      <c r="B222">
+        <v>2</v>
+      </c>
+      <c r="C222">
+        <v>2</v>
+      </c>
+      <c r="D222">
+        <v>38</v>
+      </c>
+      <c r="E222">
+        <v>105</v>
+      </c>
+      <c r="F222" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A223">
+        <v>222</v>
+      </c>
+      <c r="B223">
+        <v>0</v>
+      </c>
+      <c r="C223">
+        <v>2</v>
+      </c>
+      <c r="D223">
+        <v>176</v>
+      </c>
+      <c r="E223">
+        <v>6</v>
+      </c>
+      <c r="F223" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A224">
+        <v>223</v>
+      </c>
+      <c r="B224">
+        <v>4</v>
+      </c>
+      <c r="C224">
+        <v>4</v>
+      </c>
+      <c r="D224">
+        <v>82</v>
+      </c>
+      <c r="E224">
+        <v>41</v>
+      </c>
+      <c r="F224" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="225" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A225">
+        <v>224</v>
+      </c>
+      <c r="B225">
+        <v>4</v>
+      </c>
+      <c r="C225">
+        <v>2</v>
+      </c>
+      <c r="D225">
+        <v>90</v>
+      </c>
+      <c r="E225">
+        <v>45</v>
+      </c>
+      <c r="F225" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="226" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A226">
+        <v>225</v>
+      </c>
+      <c r="B226">
+        <v>0</v>
+      </c>
+      <c r="C226">
+        <v>2</v>
+      </c>
+      <c r="D226">
+        <v>156</v>
+      </c>
+      <c r="E226">
+        <v>16</v>
+      </c>
+      <c r="F226" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="227" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A227">
+        <v>226</v>
+      </c>
+      <c r="B227">
+        <v>0</v>
+      </c>
+      <c r="C227">
+        <v>0</v>
+      </c>
+      <c r="D227">
+        <v>132</v>
+      </c>
+      <c r="E227">
+        <v>16</v>
+      </c>
+      <c r="F227" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="228" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A228">
+        <v>227</v>
+      </c>
+      <c r="B228">
+        <v>2</v>
+      </c>
+      <c r="C228">
+        <v>2</v>
+      </c>
+      <c r="D228">
+        <v>25</v>
+      </c>
+      <c r="E228">
+        <v>98</v>
+      </c>
+      <c r="F228" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="229" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A229">
+        <v>228</v>
+      </c>
+      <c r="B229">
+        <v>2</v>
+      </c>
+      <c r="C229">
+        <v>2</v>
+      </c>
+      <c r="D229">
+        <v>21</v>
+      </c>
+      <c r="E229">
+        <v>89</v>
+      </c>
+      <c r="F229" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="230" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A230">
+        <v>229</v>
+      </c>
+      <c r="B230">
+        <v>0</v>
+      </c>
+      <c r="C230">
+        <v>0</v>
+      </c>
+      <c r="D230">
+        <v>149</v>
+      </c>
+      <c r="E230">
+        <v>22</v>
+      </c>
+      <c r="F230" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="231" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A231">
+        <v>230</v>
+      </c>
+      <c r="B231">
+        <v>0</v>
+      </c>
+      <c r="C231">
+        <v>2</v>
+      </c>
+      <c r="D231">
+        <v>189</v>
+      </c>
+      <c r="E231">
+        <v>18</v>
+      </c>
+      <c r="F231" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="232" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A232">
+        <v>231</v>
+      </c>
+      <c r="B232">
+        <v>0</v>
+      </c>
+      <c r="C232">
+        <v>2</v>
+      </c>
+      <c r="D232">
+        <v>164</v>
+      </c>
+      <c r="E232">
+        <v>16</v>
+      </c>
+      <c r="F232" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="233" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A233">
+        <v>232</v>
+      </c>
+      <c r="B233">
+        <v>4</v>
+      </c>
+      <c r="C233">
+        <v>2</v>
+      </c>
+      <c r="D233">
+        <v>45</v>
+      </c>
+      <c r="E233">
+        <v>37</v>
+      </c>
+      <c r="F233" t="s">
+        <v>4</v>
+      </c>
+      <c r="J233" s="1"/>
+    </row>
+    <row r="234" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A234">
+        <v>233</v>
+      </c>
+      <c r="B234">
+        <v>4</v>
+      </c>
+      <c r="C234">
+        <v>2</v>
+      </c>
+      <c r="D234">
+        <v>49</v>
+      </c>
+      <c r="E234">
+        <v>39</v>
+      </c>
+      <c r="F234" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="235" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A235">
+        <v>234</v>
+      </c>
+      <c r="B235">
+        <v>2</v>
+      </c>
+      <c r="C235">
+        <v>2</v>
+      </c>
+      <c r="D235">
+        <v>23</v>
+      </c>
+      <c r="E235">
+        <v>87</v>
+      </c>
+      <c r="F235" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="236" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A236">
+        <v>235</v>
+      </c>
+      <c r="B236">
+        <v>2</v>
+      </c>
+      <c r="C236">
+        <v>2</v>
+      </c>
+      <c r="D236">
+        <v>32</v>
+      </c>
+      <c r="E236">
+        <v>99</v>
+      </c>
+      <c r="F236" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="237" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A237">
+        <v>236</v>
+      </c>
+      <c r="B237">
+        <v>0</v>
+      </c>
+      <c r="C237">
+        <v>0</v>
+      </c>
+      <c r="D237">
+        <v>145</v>
+      </c>
+      <c r="E237">
+        <v>21</v>
+      </c>
+      <c r="F237" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="238" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A238">
+        <v>237</v>
+      </c>
+      <c r="B238">
+        <v>4</v>
+      </c>
+      <c r="C238">
+        <v>4</v>
+      </c>
+      <c r="D238">
+        <v>50</v>
+      </c>
+      <c r="E238">
+        <v>35</v>
+      </c>
+      <c r="F238" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="239" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A239">
+        <v>238</v>
+      </c>
+      <c r="B239">
+        <v>4</v>
+      </c>
+      <c r="C239">
+        <v>2</v>
+      </c>
+      <c r="D239">
+        <v>49</v>
+      </c>
+      <c r="E239">
+        <v>42</v>
+      </c>
+      <c r="F239" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="240" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A240">
+        <v>239</v>
+      </c>
+      <c r="B240">
+        <v>4</v>
+      </c>
+      <c r="C240">
+        <v>2</v>
+      </c>
+      <c r="D240">
+        <v>45</v>
+      </c>
+      <c r="E240">
+        <v>42</v>
+      </c>
+      <c r="F240" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="241" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A241">
+        <v>240</v>
+      </c>
+      <c r="B241">
+        <v>0</v>
+      </c>
+      <c r="C241">
+        <v>0</v>
+      </c>
+      <c r="D241">
+        <v>127</v>
+      </c>
+      <c r="E241">
+        <v>16</v>
+      </c>
+      <c r="F241" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A242">
+        <v>241</v>
+      </c>
+      <c r="B242">
+        <v>4</v>
+      </c>
+      <c r="C242">
+        <v>0</v>
+      </c>
+      <c r="D242">
+        <v>128</v>
+      </c>
+      <c r="E242">
+        <v>18</v>
+      </c>
+      <c r="F242" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="243" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A243">
+        <v>242</v>
+      </c>
+      <c r="B243">
+        <v>0</v>
+      </c>
+      <c r="C243">
+        <v>0</v>
+      </c>
+      <c r="D243">
+        <v>101</v>
+      </c>
+      <c r="E243">
+        <v>21</v>
+      </c>
+      <c r="F243" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="244" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A244">
+        <v>243</v>
+      </c>
+      <c r="B244">
+        <v>4</v>
+      </c>
+      <c r="C244">
+        <v>0</v>
+      </c>
+      <c r="D244">
+        <v>98</v>
+      </c>
+      <c r="E244">
+        <v>21</v>
+      </c>
+      <c r="F244" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="245" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A245">
+        <v>244</v>
+      </c>
+      <c r="B245">
+        <v>2</v>
+      </c>
+      <c r="C245">
+        <v>2</v>
+      </c>
+      <c r="D245">
+        <v>45</v>
+      </c>
+      <c r="E245">
+        <v>98</v>
+      </c>
+      <c r="F245" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="246" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A246">
+        <v>245</v>
+      </c>
+      <c r="B246">
+        <v>0</v>
+      </c>
+      <c r="C246">
+        <v>0</v>
+      </c>
+      <c r="D246">
+        <v>132</v>
+      </c>
+      <c r="E246">
+        <v>21</v>
+      </c>
+      <c r="F246" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="247" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A247">
+        <v>246</v>
+      </c>
+      <c r="B247">
+        <v>0</v>
+      </c>
+      <c r="C247">
+        <v>4</v>
+      </c>
+      <c r="D247">
+        <v>164</v>
+      </c>
+      <c r="E247">
+        <v>14</v>
+      </c>
+      <c r="F247" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="248" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A248">
+        <v>247</v>
+      </c>
+      <c r="B248">
+        <v>4</v>
+      </c>
+      <c r="C248">
+        <v>4</v>
+      </c>
+      <c r="D248">
+        <v>60</v>
+      </c>
+      <c r="E248">
+        <v>32</v>
+      </c>
+      <c r="F248" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="249" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A249">
+        <v>248</v>
+      </c>
+      <c r="B249">
+        <v>4</v>
+      </c>
+      <c r="C249">
+        <v>4</v>
+      </c>
+      <c r="D249">
+        <v>62</v>
+      </c>
+      <c r="E249">
+        <v>41</v>
+      </c>
+      <c r="F249" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="250" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A250">
+        <v>249</v>
+      </c>
+      <c r="B250">
+        <v>2</v>
+      </c>
+      <c r="C250">
+        <v>2</v>
+      </c>
+      <c r="D250">
+        <v>40</v>
+      </c>
+      <c r="E250">
+        <v>88</v>
+      </c>
+      <c r="F250" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="251" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A251">
+        <v>250</v>
+      </c>
+      <c r="B251">
+        <v>0</v>
+      </c>
+      <c r="C251">
+        <v>4</v>
+      </c>
+      <c r="D251">
+        <v>202</v>
+      </c>
+      <c r="E251">
+        <v>24</v>
+      </c>
+      <c r="F251" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="F1:F251" xr:uid="{94ED5614-0E0C-4455-BA1B-8CFFFEDA9206}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>